<commit_message>
Revert "ik pull die bitches"
</commit_message>
<xml_diff>
--- a/Docs/tijd_schrijven/Tijdschrijfformulier Luuk.xlsx
+++ b/Docs/tijd_schrijven/Tijdschrijfformulier Luuk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets\Docs\tijd_schrijven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8CE646-9982-4C37-95FB-CE6F881DBA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82FE6B6-98EE-4D7C-AC0D-8A6ADA7AD07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="20">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -109,15 +109,6 @@
   </si>
   <si>
     <t xml:space="preserve">Les </t>
-  </si>
-  <si>
-    <t>kbs a les</t>
-  </si>
-  <si>
-    <t>6 11 2023</t>
-  </si>
-  <si>
-    <t>les</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1157,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1178,7 +1169,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1227,20 +1218,6 @@
       </c>
       <c r="D11" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12">
-        <v>120</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1492,15 +1469,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
@@ -1508,6 +1476,15 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1531,14 +1508,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1554,4 +1523,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>